<commit_message>
reads the source excel file and creates a new excel file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,28 +14,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>World</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>oranGe</t>
+  </si>
+  <si>
+    <t>Grapes</t>
+  </si>
+  <si>
+    <t>eggplant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -63,9 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -73,49 +73,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1381125" y="762000"/>
-          <a:ext cx="4476750" cy="2238375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,14 +360,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -418,22 +372,26 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3">
-        <v>123</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
-        <v>123.456</v>
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>